<commit_message>
Manage Customer Feature Added
</commit_message>
<xml_diff>
--- a/Tasks To Complete.xlsx
+++ b/Tasks To Complete.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LOCALREPO\Learning-App-WebShopping\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="11145" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="11145"/>
   </bookViews>
   <sheets>
     <sheet name="ADMIN UI" sheetId="1" r:id="rId1"/>
@@ -13,7 +18,7 @@
     <sheet name="DEVOPS" sheetId="3" r:id="rId4"/>
     <sheet name="Automation" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -221,9 +226,6 @@
     <t>thaniga</t>
   </si>
   <si>
-    <t>christen</t>
-  </si>
-  <si>
     <t>Dhamu</t>
   </si>
   <si>
@@ -300,6 +302,9 @@
   </si>
   <si>
     <t>Pagination for pos &amp; order history</t>
+  </si>
+  <si>
+    <t>Christen</t>
   </si>
 </sst>
 </file>
@@ -322,7 +327,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -371,6 +376,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -384,7 +395,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -394,6 +405,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,6 +415,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -451,7 +466,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -486,7 +501,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -697,8 +712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A31" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,7 +741,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>8</v>
@@ -735,7 +750,7 @@
         <v>18</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -753,7 +768,7 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -804,7 +819,7 @@
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -822,7 +837,7 @@
         <v>6</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -840,7 +855,7 @@
         <v>6</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -858,7 +873,7 @@
         <v>6</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -876,7 +891,7 @@
         <v>18</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -894,7 +909,7 @@
         <v>6</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -957,7 +972,7 @@
         <v>18</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -975,7 +990,7 @@
         <v>18</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1022,7 +1037,7 @@
         <v>12</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1053,7 +1068,7 @@
         <v>18</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1070,7 +1085,7 @@
         <v>18</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1087,7 +1102,7 @@
         <v>18</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1104,7 +1119,7 @@
         <v>18</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1120,8 +1135,8 @@
       <c r="D25" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E25" s="5" t="s">
-        <v>67</v>
+      <c r="E25" s="9" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1143,7 +1158,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>38</v>
@@ -1152,7 +1167,7 @@
         <v>18</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1160,7 +1175,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>38</v>
@@ -1169,7 +1184,7 @@
         <v>18</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1177,7 +1192,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>38</v>
@@ -1186,7 +1201,7 @@
         <v>18</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1194,7 +1209,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>38</v>
@@ -1203,7 +1218,7 @@
         <v>18</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1211,7 +1226,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>38</v>
@@ -1220,7 +1235,7 @@
         <v>18</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1228,7 +1243,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>38</v>
@@ -1237,7 +1252,7 @@
         <v>18</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1245,7 +1260,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>8</v>
@@ -1254,7 +1269,7 @@
         <v>18</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1262,7 +1277,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>8</v>
@@ -1271,7 +1286,7 @@
         <v>18</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1279,7 +1294,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>8</v>
@@ -1288,7 +1303,7 @@
         <v>18</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1296,7 +1311,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>8</v>
@@ -1305,7 +1320,7 @@
         <v>18</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1313,7 +1328,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>8</v>
@@ -1322,7 +1337,7 @@
         <v>18</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1330,7 +1345,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>8</v>
@@ -1339,7 +1354,7 @@
         <v>18</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1347,7 +1362,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>8</v>
@@ -1356,7 +1371,7 @@
         <v>18</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1364,7 +1379,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>8</v>
@@ -1373,7 +1388,7 @@
         <v>18</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1381,7 +1396,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>8</v>
@@ -1390,7 +1405,7 @@
         <v>18</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1398,7 +1413,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>8</v>
@@ -1422,8 +1437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1481,7 +1496,7 @@
         <v>18</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1508,7 +1523,7 @@
         <v>18</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1535,7 +1550,7 @@
         <v>18</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1562,7 +1577,7 @@
         <v>18</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1589,7 +1604,7 @@
         <v>18</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1616,7 +1631,7 @@
         <v>18</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1643,7 +1658,7 @@
         <v>18</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1670,7 +1685,7 @@
         <v>18</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1697,7 +1712,7 @@
         <v>18</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1724,7 +1739,7 @@
         <v>18</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1751,7 +1766,7 @@
         <v>18</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1778,7 +1793,7 @@
         <v>18</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1829,12 +1844,12 @@
         <v>18</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F17" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>5</v>
@@ -1843,12 +1858,12 @@
         <v>18</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F18" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>5</v>
@@ -1859,7 +1874,7 @@
     </row>
     <row r="19" spans="6:9" x14ac:dyDescent="0.25">
       <c r="F19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G19" t="s">
         <v>5</v>
@@ -1908,7 +1923,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>8</v>
@@ -1917,7 +1932,7 @@
         <v>18</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1925,7 +1940,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>8</v>
@@ -1934,7 +1949,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1985,7 +2000,7 @@
         <v>18</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2003,7 +2018,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2021,7 +2036,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2074,7 +2089,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>42</v>
@@ -2083,7 +2098,7 @@
         <v>18</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -2096,7 +2111,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>